<commit_message>
Storey drifts plot customized
</commit_message>
<xml_diff>
--- a/Typical Input/160Wil_DES_Global.xlsx
+++ b/Typical Input/160Wil_DES_Global.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spectrum\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoftDev\RPS\Typical Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BE5F7E0-1C71-47E0-9597-1C23F73BB3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C71A907-890F-4A55-ACE7-03E5D07347B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{7553FBD0-249A-49B9-BD51-263B574C64AD}"/>
+    <workbookView xWindow="28680" yWindow="1305" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{7553FBD0-249A-49B9-BD51-263B574C64AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Joint Displacements" sheetId="1" r:id="rId1"/>
@@ -5895,8 +5895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FF27EA-046D-4639-8FD8-74D39413B731}">
   <dimension ref="A1:J267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>